<commit_message>
adding files in listview
</commit_message>
<xml_diff>
--- a/bin/Debug/net8.0-windows/93-24-2030_РКМ_Койда_1_безопасность.xlsx
+++ b/bin/Debug/net8.0-windows/93-24-2030_РКМ_Койда_1_безопасность.xlsx
@@ -1745,7 +1745,7 @@
     <x:t xml:space="preserve">(наименование организации - поставщика (подрядчика, исполнителя)) </x:t>
   </x:si>
   <x:si>
-    <x:t>цена за единицу измерения (руб.)</x:t>
+    <x:t>!*! за единицу измерения (руб.)</x:t>
   </x:si>
   <x:si>
     <x:t>ООО "Бенефит Бизнес"</x:t>
@@ -3796,7 +3796,7 @@
   </x:si>
   <x:si>
     <x:r>
-      <x:t xml:space="preserve">цена за единицу </x:t>
+      <x:t xml:space="preserve">!*! за единицу </x:t>
     </x:r>
     <x:r>
       <x:rPr>
@@ -3810,7 +3810,7 @@
   </x:si>
   <x:si>
     <x:r>
-      <x:t xml:space="preserve">цена за единицу </x:t>
+      <x:t xml:space="preserve">!*! за единицу </x:t>
     </x:r>
     <x:r>
       <x:rPr>
@@ -3992,7 +3992,7 @@
   </x:si>
   <x:si>
     <x:r>
-      <x:t xml:space="preserve">цена за единицу </x:t>
+      <x:t xml:space="preserve">!*! за единицу </x:t>
     </x:r>
     <x:r>
       <x:rPr>
@@ -4041,7 +4041,7 @@
   </x:si>
   <x:si>
     <x:r>
-      <x:t xml:space="preserve">цена за единицу </x:t>
+      <x:t xml:space="preserve">!*! за единицу </x:t>
     </x:r>
     <x:r>
       <x:rPr>

</xml_diff>